<commit_message>
Started working on doing full calculation of formula cells at the end of the import.
</commit_message>
<xml_diff>
--- a/test/xlsx/formula-simple.xlsx
+++ b/test/xlsx/formula-simple.xlsx
@@ -342,16 +342,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1">
         <f>1*2/100</f>
         <v>0.02</v>
+      </c>
+      <c r="B1">
+        <f>ROW()*COLUMN()</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <f>A1*10</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3">
+        <f>A2+B1</f>
+        <v>2.2000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oops. abs_address_t ctor takes, sheet, row and column in this order.
I got the order wrong.
</commit_message>
<xml_diff>
--- a/test/xlsx/formula-simple.xlsx
+++ b/test/xlsx/formula-simple.xlsx
@@ -355,10 +355,6 @@
         <f>1*2/100</f>
         <v>0.02</v>
       </c>
-      <c r="B1">
-        <f>ROW()*COLUMN()</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
@@ -369,7 +365,7 @@
     <row r="3" spans="1:2">
       <c r="B3">
         <f>A2+B1</f>
-        <v>2.2000000000000002</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extracted a common code block into a method.
</commit_message>
<xml_diff>
--- a/test/xlsx/formula-simple.xlsx
+++ b/test/xlsx/formula-simple.xlsx
@@ -342,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -354,6 +354,9 @@
       <c r="A1">
         <f>1*2/100</f>
         <v>0.02</v>
+      </c>
+      <c r="B1">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -365,7 +368,13 @@
     <row r="3" spans="1:2">
       <c r="B3">
         <f>A2+B1</f>
-        <v>0.2</v>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <f>SUM(A1:B3)</f>
+        <v>26.419999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more non-shared formulas.
</commit_message>
<xml_diff>
--- a/test/xlsx/formula-simple.xlsx
+++ b/test/xlsx/formula-simple.xlsx
@@ -342,15 +342,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:10">
       <c r="A1">
         <f>1*2/100</f>
         <v>0.02</v>
@@ -359,22 +359,81 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <f>A1*10</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:10">
       <c r="B3">
         <f>A2+B1</f>
         <v>13.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <f>SUM(A1:B3)</f>
         <v>26.419999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8">
+        <f>A7+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="C9">
+        <f>B8+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="D10">
+        <f>C9+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="E11">
+        <f>D10+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="F12">
+        <f>E11+1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="G13">
+        <f>F12+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="H14">
+        <f>G13+1</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="I15">
+        <f>H14+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="J16">
+        <f>I15+1</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>